<commit_message>
fix: nist csf 2.0 scores localization
</commit_message>
<xml_diff>
--- a/tools/excel/nist/nist-csf-2.0.xlsx
+++ b/tools/excel/nist/nist-csf-2.0.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10329"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10608"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ericlaubacher/Documents/GitHub/ciso-assistant-community/tools/nist/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nassim/Dev/intuitem/ciso-assistant-community/tools/excel/nist/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{348EC931-B4B2-0F44-A863-998E6F389A15}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DEA69950-017B-C54B-B418-F1FA48692F7A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="20360" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="21580" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="library_content" sheetId="2" r:id="rId1"/>
@@ -19,13 +19,14 @@
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">csf!$A$1:$L$135</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">library_content!$A$1:$C$21</definedName>
   </definedNames>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1128" uniqueCount="1012">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1128" uniqueCount="1010">
   <si>
     <t>assessable</t>
   </si>
@@ -2949,12 +2950,6 @@
   </si>
   <si>
     <t>Les mises à jour publiques sur la récupération après incident sont partagées à l’aide de méthodes et de messages approuvés.</t>
-  </si>
-  <si>
-    <t>name[sp]</t>
-  </si>
-  <si>
-    <t>description[sp]</t>
   </si>
   <si>
     <t>GOBERNAR</t>
@@ -4310,7 +4305,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -4632,7 +4627,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6663DDE6-1E5F-334B-86D6-FF0D04872286}">
   <dimension ref="A1:C21"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" zoomScale="231" workbookViewId="0">
+    <sheetView topLeftCell="A4" workbookViewId="0">
       <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
@@ -4795,7 +4790,7 @@
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>995</v>
+        <v>993</v>
       </c>
       <c r="B19" s="1" t="s">
         <v>446</v>
@@ -4803,7 +4798,7 @@
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>996</v>
+        <v>994</v>
       </c>
       <c r="B20" s="1" t="s">
         <v>431</v>
@@ -4811,13 +4806,14 @@
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>997</v>
+        <v>995</v>
       </c>
       <c r="B21" s="1" t="s">
         <v>446</v>
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:C21" xr:uid="{6663DDE6-1E5F-334B-86D6-FF0D04872286}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -4826,8 +4822,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L135"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="125" workbookViewId="0">
-      <selection activeCell="H136" sqref="H136"/>
+    <sheetView topLeftCell="K3" zoomScale="125" workbookViewId="0">
+      <selection activeCell="K7" sqref="K7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -4873,13 +4869,13 @@
         <v>603</v>
       </c>
       <c r="J1" s="6" t="s">
+        <v>996</v>
+      </c>
+      <c r="K1" s="7" t="s">
+        <v>997</v>
+      </c>
+      <c r="L1" s="8" t="s">
         <v>998</v>
-      </c>
-      <c r="K1" s="7" t="s">
-        <v>999</v>
-      </c>
-      <c r="L1" s="8" t="s">
-        <v>1000</v>
       </c>
     </row>
     <row r="2" spans="1:12" ht="32" x14ac:dyDescent="0.2">
@@ -4902,10 +4898,10 @@
         <v>461</v>
       </c>
       <c r="J2" s="2" t="s">
-        <v>719</v>
+        <v>717</v>
       </c>
       <c r="K2" t="s">
-        <v>720</v>
+        <v>718</v>
       </c>
     </row>
     <row r="3" spans="1:12" ht="48" x14ac:dyDescent="0.2">
@@ -4928,10 +4924,10 @@
         <v>491</v>
       </c>
       <c r="J3" s="2" t="s">
-        <v>721</v>
+        <v>719</v>
       </c>
       <c r="K3" t="s">
-        <v>722</v>
+        <v>720</v>
       </c>
     </row>
     <row r="4" spans="1:12" ht="80" customHeight="1" x14ac:dyDescent="0.2">
@@ -4958,10 +4954,10 @@
         <v>497</v>
       </c>
       <c r="K4" t="s">
-        <v>723</v>
+        <v>721</v>
       </c>
       <c r="L4" s="2" t="s">
-        <v>724</v>
+        <v>722</v>
       </c>
     </row>
     <row r="5" spans="1:12" ht="176" customHeight="1" x14ac:dyDescent="0.2">
@@ -4988,10 +4984,10 @@
         <v>498</v>
       </c>
       <c r="K5" t="s">
-        <v>725</v>
+        <v>723</v>
       </c>
       <c r="L5" s="2" t="s">
-        <v>726</v>
+        <v>724</v>
       </c>
     </row>
     <row r="6" spans="1:12" ht="208" customHeight="1" x14ac:dyDescent="0.2">
@@ -5018,10 +5014,10 @@
         <v>499</v>
       </c>
       <c r="K6" t="s">
-        <v>727</v>
+        <v>725</v>
       </c>
       <c r="L6" s="2" t="s">
-        <v>728</v>
+        <v>726</v>
       </c>
     </row>
     <row r="7" spans="1:12" ht="208" customHeight="1" x14ac:dyDescent="0.2">
@@ -5048,10 +5044,10 @@
         <v>500</v>
       </c>
       <c r="K7" t="s">
-        <v>729</v>
+        <v>727</v>
       </c>
       <c r="L7" s="2" t="s">
-        <v>730</v>
+        <v>728</v>
       </c>
     </row>
     <row r="8" spans="1:12" ht="144" customHeight="1" x14ac:dyDescent="0.2">
@@ -5078,10 +5074,10 @@
         <v>501</v>
       </c>
       <c r="K8" t="s">
-        <v>731</v>
+        <v>729</v>
       </c>
       <c r="L8" s="2" t="s">
-        <v>732</v>
+        <v>730</v>
       </c>
     </row>
     <row r="9" spans="1:12" ht="48" x14ac:dyDescent="0.2">
@@ -5104,10 +5100,10 @@
         <v>492</v>
       </c>
       <c r="J9" s="2" t="s">
-        <v>733</v>
+        <v>731</v>
       </c>
       <c r="K9" t="s">
-        <v>734</v>
+        <v>732</v>
       </c>
     </row>
     <row r="10" spans="1:12" ht="176" customHeight="1" x14ac:dyDescent="0.2">
@@ -5134,10 +5130,10 @@
         <v>502</v>
       </c>
       <c r="K10" t="s">
-        <v>735</v>
+        <v>733</v>
       </c>
       <c r="L10" s="2" t="s">
-        <v>736</v>
+        <v>734</v>
       </c>
     </row>
     <row r="11" spans="1:12" ht="176" customHeight="1" x14ac:dyDescent="0.2">
@@ -5164,10 +5160,10 @@
         <v>503</v>
       </c>
       <c r="K11" t="s">
-        <v>737</v>
+        <v>735</v>
       </c>
       <c r="L11" s="2" t="s">
-        <v>738</v>
+        <v>736</v>
       </c>
     </row>
     <row r="12" spans="1:12" ht="128" customHeight="1" x14ac:dyDescent="0.2">
@@ -5194,10 +5190,10 @@
         <v>504</v>
       </c>
       <c r="K12" t="s">
-        <v>739</v>
+        <v>737</v>
       </c>
       <c r="L12" s="2" t="s">
-        <v>740</v>
+        <v>738</v>
       </c>
     </row>
     <row r="13" spans="1:12" ht="160" customHeight="1" x14ac:dyDescent="0.2">
@@ -5224,10 +5220,10 @@
         <v>505</v>
       </c>
       <c r="K13" t="s">
-        <v>741</v>
+        <v>739</v>
       </c>
       <c r="L13" s="2" t="s">
-        <v>742</v>
+        <v>740</v>
       </c>
     </row>
     <row r="14" spans="1:12" ht="160" customHeight="1" x14ac:dyDescent="0.2">
@@ -5254,10 +5250,10 @@
         <v>506</v>
       </c>
       <c r="K14" t="s">
-        <v>743</v>
+        <v>741</v>
       </c>
       <c r="L14" s="2" t="s">
-        <v>744</v>
+        <v>742</v>
       </c>
     </row>
     <row r="15" spans="1:12" ht="192" customHeight="1" x14ac:dyDescent="0.2">
@@ -5284,10 +5280,10 @@
         <v>507</v>
       </c>
       <c r="K15" t="s">
-        <v>745</v>
+        <v>743</v>
       </c>
       <c r="L15" s="2" t="s">
-        <v>746</v>
+        <v>744</v>
       </c>
     </row>
     <row r="16" spans="1:12" ht="128" customHeight="1" x14ac:dyDescent="0.2">
@@ -5314,10 +5310,10 @@
         <v>508</v>
       </c>
       <c r="K16" t="s">
-        <v>747</v>
+        <v>745</v>
       </c>
       <c r="L16" s="2" t="s">
-        <v>748</v>
+        <v>746</v>
       </c>
     </row>
     <row r="17" spans="1:12" ht="32" x14ac:dyDescent="0.2">
@@ -5340,10 +5336,10 @@
         <v>493</v>
       </c>
       <c r="J17" s="2" t="s">
-        <v>749</v>
+        <v>747</v>
       </c>
       <c r="K17" t="s">
-        <v>750</v>
+        <v>748</v>
       </c>
     </row>
     <row r="18" spans="1:12" ht="224" customHeight="1" x14ac:dyDescent="0.2">
@@ -5370,10 +5366,10 @@
         <v>509</v>
       </c>
       <c r="K18" t="s">
-        <v>751</v>
+        <v>749</v>
       </c>
       <c r="L18" s="2" t="s">
-        <v>752</v>
+        <v>750</v>
       </c>
     </row>
     <row r="19" spans="1:12" ht="240" customHeight="1" x14ac:dyDescent="0.2">
@@ -5400,10 +5396,10 @@
         <v>510</v>
       </c>
       <c r="K19" t="s">
-        <v>753</v>
+        <v>751</v>
       </c>
       <c r="L19" s="2" t="s">
-        <v>754</v>
+        <v>752</v>
       </c>
     </row>
     <row r="20" spans="1:12" ht="160" customHeight="1" x14ac:dyDescent="0.2">
@@ -5430,10 +5426,10 @@
         <v>511</v>
       </c>
       <c r="K20" t="s">
-        <v>755</v>
+        <v>753</v>
       </c>
       <c r="L20" s="2" t="s">
-        <v>756</v>
+        <v>754</v>
       </c>
     </row>
     <row r="21" spans="1:12" ht="208" customHeight="1" x14ac:dyDescent="0.2">
@@ -5460,10 +5456,10 @@
         <v>512</v>
       </c>
       <c r="K21" t="s">
-        <v>757</v>
+        <v>755</v>
       </c>
       <c r="L21" s="2" t="s">
-        <v>758</v>
+        <v>756</v>
       </c>
     </row>
     <row r="22" spans="1:12" ht="16" x14ac:dyDescent="0.2">
@@ -5486,10 +5482,10 @@
         <v>494</v>
       </c>
       <c r="J22" s="2" t="s">
-        <v>759</v>
+        <v>757</v>
       </c>
       <c r="K22" t="s">
-        <v>760</v>
+        <v>758</v>
       </c>
     </row>
     <row r="23" spans="1:12" ht="272" customHeight="1" x14ac:dyDescent="0.2">
@@ -5516,10 +5512,10 @@
         <v>513</v>
       </c>
       <c r="K23" t="s">
-        <v>761</v>
+        <v>759</v>
       </c>
       <c r="L23" s="2" t="s">
-        <v>762</v>
+        <v>760</v>
       </c>
     </row>
     <row r="24" spans="1:12" ht="240" customHeight="1" x14ac:dyDescent="0.2">
@@ -5546,10 +5542,10 @@
         <v>514</v>
       </c>
       <c r="K24" t="s">
-        <v>763</v>
+        <v>761</v>
       </c>
       <c r="L24" s="2" t="s">
-        <v>764</v>
+        <v>762</v>
       </c>
     </row>
     <row r="25" spans="1:12" ht="32" x14ac:dyDescent="0.2">
@@ -5572,10 +5568,10 @@
         <v>495</v>
       </c>
       <c r="J25" s="2" t="s">
-        <v>765</v>
+        <v>763</v>
       </c>
       <c r="K25" t="s">
-        <v>766</v>
+        <v>764</v>
       </c>
     </row>
     <row r="26" spans="1:12" ht="96" customHeight="1" x14ac:dyDescent="0.2">
@@ -5602,10 +5598,10 @@
         <v>515</v>
       </c>
       <c r="K26" t="s">
-        <v>767</v>
+        <v>765</v>
       </c>
       <c r="L26" s="2" t="s">
-        <v>768</v>
+        <v>766</v>
       </c>
     </row>
     <row r="27" spans="1:12" ht="128" customHeight="1" x14ac:dyDescent="0.2">
@@ -5632,10 +5628,10 @@
         <v>516</v>
       </c>
       <c r="K27" t="s">
-        <v>769</v>
+        <v>767</v>
       </c>
       <c r="L27" s="2" t="s">
-        <v>770</v>
+        <v>768</v>
       </c>
     </row>
     <row r="28" spans="1:12" ht="144" customHeight="1" x14ac:dyDescent="0.2">
@@ -5662,10 +5658,10 @@
         <v>517</v>
       </c>
       <c r="K28" t="s">
-        <v>771</v>
+        <v>769</v>
       </c>
       <c r="L28" s="2" t="s">
-        <v>772</v>
+        <v>770</v>
       </c>
     </row>
     <row r="29" spans="1:12" ht="48" x14ac:dyDescent="0.2">
@@ -5688,10 +5684,10 @@
         <v>496</v>
       </c>
       <c r="J29" s="2" t="s">
-        <v>773</v>
+        <v>771</v>
       </c>
       <c r="K29" t="s">
-        <v>774</v>
+        <v>772</v>
       </c>
     </row>
     <row r="30" spans="1:12" ht="304" customHeight="1" x14ac:dyDescent="0.2">
@@ -5718,10 +5714,10 @@
         <v>518</v>
       </c>
       <c r="K30" t="s">
-        <v>775</v>
+        <v>773</v>
       </c>
       <c r="L30" s="2" t="s">
-        <v>776</v>
+        <v>774</v>
       </c>
     </row>
     <row r="31" spans="1:12" ht="409.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -5748,10 +5744,10 @@
         <v>519</v>
       </c>
       <c r="K31" t="s">
-        <v>777</v>
+        <v>775</v>
       </c>
       <c r="L31" s="2" t="s">
-        <v>778</v>
+        <v>776</v>
       </c>
     </row>
     <row r="32" spans="1:12" ht="176" customHeight="1" x14ac:dyDescent="0.2">
@@ -5778,10 +5774,10 @@
         <v>520</v>
       </c>
       <c r="K32" t="s">
-        <v>779</v>
+        <v>777</v>
       </c>
       <c r="L32" s="2" t="s">
-        <v>780</v>
+        <v>778</v>
       </c>
     </row>
     <row r="33" spans="1:12" ht="128" customHeight="1" x14ac:dyDescent="0.2">
@@ -5808,10 +5804,10 @@
         <v>521</v>
       </c>
       <c r="K33" t="s">
-        <v>781</v>
+        <v>779</v>
       </c>
       <c r="L33" s="2" t="s">
-        <v>782</v>
+        <v>780</v>
       </c>
     </row>
     <row r="34" spans="1:12" ht="409.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -5838,10 +5834,10 @@
         <v>522</v>
       </c>
       <c r="K34" t="s">
-        <v>783</v>
+        <v>781</v>
       </c>
       <c r="L34" s="2" t="s">
-        <v>784</v>
+        <v>782</v>
       </c>
     </row>
     <row r="35" spans="1:12" ht="192" customHeight="1" x14ac:dyDescent="0.2">
@@ -5868,10 +5864,10 @@
         <v>523</v>
       </c>
       <c r="K35" t="s">
-        <v>785</v>
+        <v>783</v>
       </c>
       <c r="L35" s="2" t="s">
-        <v>786</v>
+        <v>784</v>
       </c>
     </row>
     <row r="36" spans="1:12" ht="288" customHeight="1" x14ac:dyDescent="0.2">
@@ -5898,10 +5894,10 @@
         <v>524</v>
       </c>
       <c r="K36" t="s">
-        <v>787</v>
+        <v>785</v>
       </c>
       <c r="L36" s="2" t="s">
-        <v>788</v>
+        <v>786</v>
       </c>
     </row>
     <row r="37" spans="1:12" ht="224" customHeight="1" x14ac:dyDescent="0.2">
@@ -5928,10 +5924,10 @@
         <v>525</v>
       </c>
       <c r="K37" t="s">
-        <v>789</v>
+        <v>787</v>
       </c>
       <c r="L37" s="2" t="s">
-        <v>790</v>
+        <v>788</v>
       </c>
     </row>
     <row r="38" spans="1:12" ht="240" customHeight="1" x14ac:dyDescent="0.2">
@@ -5958,10 +5954,10 @@
         <v>526</v>
       </c>
       <c r="K38" t="s">
-        <v>791</v>
+        <v>789</v>
       </c>
       <c r="L38" s="2" t="s">
-        <v>792</v>
+        <v>790</v>
       </c>
     </row>
     <row r="39" spans="1:12" ht="288" customHeight="1" x14ac:dyDescent="0.2">
@@ -5988,10 +5984,10 @@
         <v>527</v>
       </c>
       <c r="K39" t="s">
-        <v>793</v>
+        <v>791</v>
       </c>
       <c r="L39" s="2" t="s">
-        <v>794</v>
+        <v>792</v>
       </c>
     </row>
     <row r="40" spans="1:12" ht="16" x14ac:dyDescent="0.2">
@@ -6014,10 +6010,10 @@
         <v>459</v>
       </c>
       <c r="J40" s="2" t="s">
-        <v>795</v>
+        <v>793</v>
       </c>
       <c r="K40" t="s">
-        <v>796</v>
+        <v>794</v>
       </c>
     </row>
     <row r="41" spans="1:12" ht="48" x14ac:dyDescent="0.2">
@@ -6040,10 +6036,10 @@
         <v>637</v>
       </c>
       <c r="J41" s="2" t="s">
-        <v>797</v>
+        <v>795</v>
       </c>
       <c r="K41" t="s">
-        <v>798</v>
+        <v>796</v>
       </c>
     </row>
     <row r="42" spans="1:12" ht="80" customHeight="1" x14ac:dyDescent="0.2">
@@ -6070,10 +6066,10 @@
         <v>528</v>
       </c>
       <c r="K42" t="s">
-        <v>799</v>
+        <v>797</v>
       </c>
       <c r="L42" s="2" t="s">
-        <v>800</v>
+        <v>798</v>
       </c>
     </row>
     <row r="43" spans="1:12" ht="144" customHeight="1" x14ac:dyDescent="0.2">
@@ -6100,10 +6096,10 @@
         <v>529</v>
       </c>
       <c r="K43" t="s">
-        <v>801</v>
+        <v>799</v>
       </c>
       <c r="L43" s="2" t="s">
-        <v>802</v>
+        <v>800</v>
       </c>
     </row>
     <row r="44" spans="1:12" ht="208" customHeight="1" x14ac:dyDescent="0.2">
@@ -6130,10 +6126,10 @@
         <v>530</v>
       </c>
       <c r="K44" t="s">
-        <v>803</v>
+        <v>801</v>
       </c>
       <c r="L44" s="2" t="s">
-        <v>804</v>
+        <v>802</v>
       </c>
     </row>
     <row r="45" spans="1:12" ht="160" customHeight="1" x14ac:dyDescent="0.2">
@@ -6160,10 +6156,10 @@
         <v>531</v>
       </c>
       <c r="K45" t="s">
-        <v>805</v>
+        <v>803</v>
       </c>
       <c r="L45" s="2" t="s">
-        <v>806</v>
+        <v>804</v>
       </c>
     </row>
     <row r="46" spans="1:12" ht="96" customHeight="1" x14ac:dyDescent="0.2">
@@ -6190,10 +6186,10 @@
         <v>532</v>
       </c>
       <c r="K46" t="s">
-        <v>807</v>
+        <v>805</v>
       </c>
       <c r="L46" s="2" t="s">
-        <v>808</v>
+        <v>806</v>
       </c>
     </row>
     <row r="47" spans="1:12" ht="192" customHeight="1" x14ac:dyDescent="0.2">
@@ -6220,10 +6216,10 @@
         <v>533</v>
       </c>
       <c r="K47" t="s">
-        <v>809</v>
+        <v>807</v>
       </c>
       <c r="L47" s="2" t="s">
-        <v>810</v>
+        <v>808</v>
       </c>
     </row>
     <row r="48" spans="1:12" ht="409.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -6250,10 +6246,10 @@
         <v>534</v>
       </c>
       <c r="K48" t="s">
-        <v>811</v>
+        <v>809</v>
       </c>
       <c r="L48" s="2" t="s">
-        <v>812</v>
+        <v>810</v>
       </c>
     </row>
     <row r="49" spans="1:12" ht="32" x14ac:dyDescent="0.2">
@@ -6273,13 +6269,13 @@
         <v>473</v>
       </c>
       <c r="H49" s="2" t="s">
-        <v>1001</v>
+        <v>999</v>
       </c>
       <c r="J49" s="2" t="s">
-        <v>813</v>
+        <v>811</v>
       </c>
       <c r="K49" t="s">
-        <v>814</v>
+        <v>812</v>
       </c>
     </row>
     <row r="50" spans="1:12" ht="256" customHeight="1" x14ac:dyDescent="0.2">
@@ -6306,10 +6302,10 @@
         <v>535</v>
       </c>
       <c r="K50" t="s">
-        <v>815</v>
+        <v>813</v>
       </c>
       <c r="L50" s="2" t="s">
-        <v>816</v>
+        <v>814</v>
       </c>
     </row>
     <row r="51" spans="1:12" ht="160" customHeight="1" x14ac:dyDescent="0.2">
@@ -6336,10 +6332,10 @@
         <v>536</v>
       </c>
       <c r="K51" t="s">
-        <v>817</v>
+        <v>815</v>
       </c>
       <c r="L51" s="2" t="s">
-        <v>818</v>
+        <v>816</v>
       </c>
     </row>
     <row r="52" spans="1:12" ht="144" customHeight="1" x14ac:dyDescent="0.2">
@@ -6366,10 +6362,10 @@
         <v>537</v>
       </c>
       <c r="K52" t="s">
-        <v>819</v>
+        <v>817</v>
       </c>
       <c r="L52" s="2" t="s">
-        <v>820</v>
+        <v>818</v>
       </c>
     </row>
     <row r="53" spans="1:12" ht="176" customHeight="1" x14ac:dyDescent="0.2">
@@ -6396,10 +6392,10 @@
         <v>538</v>
       </c>
       <c r="K53" t="s">
-        <v>821</v>
+        <v>819</v>
       </c>
       <c r="L53" s="2" t="s">
-        <v>822</v>
+        <v>820</v>
       </c>
     </row>
     <row r="54" spans="1:12" ht="80" customHeight="1" x14ac:dyDescent="0.2">
@@ -6426,10 +6422,10 @@
         <v>539</v>
       </c>
       <c r="K54" t="s">
-        <v>823</v>
+        <v>821</v>
       </c>
       <c r="L54" s="2" t="s">
-        <v>824</v>
+        <v>822</v>
       </c>
     </row>
     <row r="55" spans="1:12" ht="208" customHeight="1" x14ac:dyDescent="0.2">
@@ -6456,10 +6452,10 @@
         <v>540</v>
       </c>
       <c r="K55" t="s">
-        <v>825</v>
+        <v>823</v>
       </c>
       <c r="L55" s="2" t="s">
-        <v>826</v>
+        <v>824</v>
       </c>
     </row>
     <row r="56" spans="1:12" ht="160" customHeight="1" x14ac:dyDescent="0.2">
@@ -6486,10 +6482,10 @@
         <v>541</v>
       </c>
       <c r="K56" t="s">
-        <v>827</v>
+        <v>825</v>
       </c>
       <c r="L56" s="2" t="s">
-        <v>828</v>
+        <v>826</v>
       </c>
     </row>
     <row r="57" spans="1:12" ht="160" customHeight="1" x14ac:dyDescent="0.2">
@@ -6516,10 +6512,10 @@
         <v>542</v>
       </c>
       <c r="K57" t="s">
-        <v>829</v>
+        <v>827</v>
       </c>
       <c r="L57" s="2" t="s">
-        <v>830</v>
+        <v>828</v>
       </c>
     </row>
     <row r="58" spans="1:12" ht="64" customHeight="1" x14ac:dyDescent="0.2">
@@ -6546,10 +6542,10 @@
         <v>543</v>
       </c>
       <c r="K58" t="s">
-        <v>831</v>
+        <v>829</v>
       </c>
       <c r="L58" s="2" t="s">
-        <v>832</v>
+        <v>830</v>
       </c>
     </row>
     <row r="59" spans="1:12" ht="48" customHeight="1" x14ac:dyDescent="0.2">
@@ -6576,10 +6572,10 @@
         <v>544</v>
       </c>
       <c r="K59" t="s">
-        <v>833</v>
+        <v>831</v>
       </c>
       <c r="L59" s="2" t="s">
-        <v>834</v>
+        <v>832</v>
       </c>
     </row>
     <row r="60" spans="1:12" ht="32" x14ac:dyDescent="0.2">
@@ -6599,13 +6595,13 @@
         <v>472</v>
       </c>
       <c r="H60" s="2" t="s">
-        <v>1003</v>
+        <v>1001</v>
       </c>
       <c r="J60" s="2" t="s">
-        <v>835</v>
+        <v>833</v>
       </c>
       <c r="K60" t="s">
-        <v>836</v>
+        <v>834</v>
       </c>
     </row>
     <row r="61" spans="1:12" ht="144" customHeight="1" x14ac:dyDescent="0.2">
@@ -6632,10 +6628,10 @@
         <v>545</v>
       </c>
       <c r="K61" t="s">
-        <v>837</v>
+        <v>835</v>
       </c>
       <c r="L61" s="2" t="s">
-        <v>838</v>
+        <v>836</v>
       </c>
     </row>
     <row r="62" spans="1:12" ht="365" customHeight="1" x14ac:dyDescent="0.2">
@@ -6662,10 +6658,10 @@
         <v>546</v>
       </c>
       <c r="K62" t="s">
-        <v>839</v>
+        <v>837</v>
       </c>
       <c r="L62" s="2" t="s">
-        <v>840</v>
+        <v>838</v>
       </c>
     </row>
     <row r="63" spans="1:12" ht="112" customHeight="1" x14ac:dyDescent="0.2">
@@ -6692,10 +6688,10 @@
         <v>547</v>
       </c>
       <c r="K63" t="s">
-        <v>841</v>
+        <v>839</v>
       </c>
       <c r="L63" s="2" t="s">
-        <v>842</v>
+        <v>840</v>
       </c>
     </row>
     <row r="64" spans="1:12" ht="320" customHeight="1" x14ac:dyDescent="0.2">
@@ -6722,10 +6718,10 @@
         <v>548</v>
       </c>
       <c r="K64" t="s">
-        <v>843</v>
+        <v>841</v>
       </c>
       <c r="L64" s="2" t="s">
-        <v>844</v>
+        <v>842</v>
       </c>
     </row>
     <row r="65" spans="1:12" ht="16" x14ac:dyDescent="0.2">
@@ -6748,10 +6744,10 @@
         <v>462</v>
       </c>
       <c r="J65" s="2" t="s">
-        <v>845</v>
+        <v>843</v>
       </c>
       <c r="K65" t="s">
-        <v>846</v>
+        <v>844</v>
       </c>
     </row>
     <row r="66" spans="1:12" ht="32" x14ac:dyDescent="0.2">
@@ -6774,10 +6770,10 @@
         <v>659</v>
       </c>
       <c r="J66" s="2" t="s">
-        <v>847</v>
+        <v>845</v>
       </c>
       <c r="K66" t="s">
-        <v>848</v>
+        <v>846</v>
       </c>
     </row>
     <row r="67" spans="1:12" ht="208" customHeight="1" x14ac:dyDescent="0.2">
@@ -6804,10 +6800,10 @@
         <v>549</v>
       </c>
       <c r="K67" t="s">
-        <v>849</v>
+        <v>847</v>
       </c>
       <c r="L67" s="2" t="s">
-        <v>850</v>
+        <v>848</v>
       </c>
     </row>
     <row r="68" spans="1:12" ht="112" customHeight="1" x14ac:dyDescent="0.2">
@@ -6834,10 +6830,10 @@
         <v>550</v>
       </c>
       <c r="K68" t="s">
-        <v>851</v>
+        <v>849</v>
       </c>
       <c r="L68" s="2" t="s">
-        <v>852</v>
+        <v>850</v>
       </c>
     </row>
     <row r="69" spans="1:12" ht="144" customHeight="1" x14ac:dyDescent="0.2">
@@ -6864,10 +6860,10 @@
         <v>551</v>
       </c>
       <c r="K69" t="s">
-        <v>853</v>
+        <v>851</v>
       </c>
       <c r="L69" s="2" t="s">
-        <v>854</v>
+        <v>852</v>
       </c>
     </row>
     <row r="70" spans="1:12" ht="192" customHeight="1" x14ac:dyDescent="0.2">
@@ -6894,10 +6890,10 @@
         <v>552</v>
       </c>
       <c r="K70" t="s">
-        <v>855</v>
+        <v>853</v>
       </c>
       <c r="L70" s="2" t="s">
-        <v>856</v>
+        <v>854</v>
       </c>
     </row>
     <row r="71" spans="1:12" ht="224" customHeight="1" x14ac:dyDescent="0.2">
@@ -6924,10 +6920,10 @@
         <v>553</v>
       </c>
       <c r="K71" t="s">
-        <v>857</v>
+        <v>855</v>
       </c>
       <c r="L71" s="2" t="s">
-        <v>858</v>
+        <v>856</v>
       </c>
     </row>
     <row r="72" spans="1:12" ht="144" customHeight="1" x14ac:dyDescent="0.2">
@@ -6954,10 +6950,10 @@
         <v>554</v>
       </c>
       <c r="K72" t="s">
-        <v>859</v>
+        <v>857</v>
       </c>
       <c r="L72" s="2" t="s">
-        <v>860</v>
+        <v>858</v>
       </c>
     </row>
     <row r="73" spans="1:12" ht="32" x14ac:dyDescent="0.2">
@@ -6977,13 +6973,13 @@
         <v>474</v>
       </c>
       <c r="H73" s="2" t="s">
-        <v>1002</v>
+        <v>1000</v>
       </c>
       <c r="J73" s="2" t="s">
-        <v>861</v>
+        <v>859</v>
       </c>
       <c r="K73" t="s">
-        <v>862</v>
+        <v>860</v>
       </c>
     </row>
     <row r="74" spans="1:12" ht="256" customHeight="1" x14ac:dyDescent="0.2">
@@ -7010,10 +7006,10 @@
         <v>555</v>
       </c>
       <c r="K74" t="s">
-        <v>863</v>
+        <v>861</v>
       </c>
       <c r="L74" s="2" t="s">
-        <v>864</v>
+        <v>862</v>
       </c>
     </row>
     <row r="75" spans="1:12" ht="240" customHeight="1" x14ac:dyDescent="0.2">
@@ -7040,10 +7036,10 @@
         <v>556</v>
       </c>
       <c r="K75" t="s">
-        <v>865</v>
+        <v>863</v>
       </c>
       <c r="L75" s="2" t="s">
-        <v>866</v>
+        <v>864</v>
       </c>
     </row>
     <row r="76" spans="1:12" ht="32" x14ac:dyDescent="0.2">
@@ -7063,13 +7059,13 @@
         <v>479</v>
       </c>
       <c r="H76" s="2" t="s">
-        <v>1004</v>
+        <v>1002</v>
       </c>
       <c r="J76" s="2" t="s">
-        <v>867</v>
+        <v>865</v>
       </c>
       <c r="K76" t="s">
-        <v>868</v>
+        <v>866</v>
       </c>
     </row>
     <row r="77" spans="1:12" ht="240" customHeight="1" x14ac:dyDescent="0.2">
@@ -7096,10 +7092,10 @@
         <v>557</v>
       </c>
       <c r="K77" t="s">
-        <v>869</v>
+        <v>867</v>
       </c>
       <c r="L77" s="2" t="s">
-        <v>870</v>
+        <v>868</v>
       </c>
     </row>
     <row r="78" spans="1:12" ht="224" customHeight="1" x14ac:dyDescent="0.2">
@@ -7126,10 +7122,10 @@
         <v>558</v>
       </c>
       <c r="K78" t="s">
-        <v>871</v>
+        <v>869</v>
       </c>
       <c r="L78" s="2" t="s">
-        <v>872</v>
+        <v>870</v>
       </c>
     </row>
     <row r="79" spans="1:12" ht="96" customHeight="1" x14ac:dyDescent="0.2">
@@ -7156,10 +7152,10 @@
         <v>559</v>
       </c>
       <c r="K79" t="s">
-        <v>873</v>
+        <v>871</v>
       </c>
       <c r="L79" s="2" t="s">
-        <v>874</v>
+        <v>872</v>
       </c>
     </row>
     <row r="80" spans="1:12" ht="160" customHeight="1" x14ac:dyDescent="0.2">
@@ -7186,10 +7182,10 @@
         <v>560</v>
       </c>
       <c r="K80" t="s">
-        <v>875</v>
+        <v>873</v>
       </c>
       <c r="L80" s="2" t="s">
-        <v>876</v>
+        <v>874</v>
       </c>
     </row>
     <row r="81" spans="1:12" ht="48" x14ac:dyDescent="0.2">
@@ -7209,13 +7205,13 @@
         <v>478</v>
       </c>
       <c r="H81" s="2" t="s">
-        <v>1005</v>
+        <v>1003</v>
       </c>
       <c r="J81" s="2" t="s">
-        <v>877</v>
+        <v>875</v>
       </c>
       <c r="K81" t="s">
-        <v>878</v>
+        <v>876</v>
       </c>
     </row>
     <row r="82" spans="1:12" ht="160" customHeight="1" x14ac:dyDescent="0.2">
@@ -7242,10 +7238,10 @@
         <v>561</v>
       </c>
       <c r="K82" t="s">
-        <v>879</v>
+        <v>877</v>
       </c>
       <c r="L82" s="2" t="s">
-        <v>880</v>
+        <v>878</v>
       </c>
     </row>
     <row r="83" spans="1:12" ht="272" customHeight="1" x14ac:dyDescent="0.2">
@@ -7272,10 +7268,10 @@
         <v>562</v>
       </c>
       <c r="K83" t="s">
-        <v>881</v>
+        <v>879</v>
       </c>
       <c r="L83" s="2" t="s">
-        <v>882</v>
+        <v>880</v>
       </c>
     </row>
     <row r="84" spans="1:12" ht="144" customHeight="1" x14ac:dyDescent="0.2">
@@ -7302,10 +7298,10 @@
         <v>563</v>
       </c>
       <c r="K84" t="s">
-        <v>883</v>
+        <v>881</v>
       </c>
       <c r="L84" s="2" t="s">
-        <v>884</v>
+        <v>882</v>
       </c>
     </row>
     <row r="85" spans="1:12" ht="144" customHeight="1" x14ac:dyDescent="0.2">
@@ -7332,10 +7328,10 @@
         <v>564</v>
       </c>
       <c r="K85" t="s">
-        <v>885</v>
+        <v>883</v>
       </c>
       <c r="L85" s="2" t="s">
-        <v>886</v>
+        <v>884</v>
       </c>
     </row>
     <row r="86" spans="1:12" ht="160" customHeight="1" x14ac:dyDescent="0.2">
@@ -7362,10 +7358,10 @@
         <v>565</v>
       </c>
       <c r="K86" t="s">
-        <v>887</v>
+        <v>885</v>
       </c>
       <c r="L86" s="2" t="s">
-        <v>888</v>
+        <v>886</v>
       </c>
     </row>
     <row r="87" spans="1:12" ht="128" customHeight="1" x14ac:dyDescent="0.2">
@@ -7392,10 +7388,10 @@
         <v>566</v>
       </c>
       <c r="K87" t="s">
-        <v>889</v>
+        <v>887</v>
       </c>
       <c r="L87" s="2" t="s">
-        <v>890</v>
+        <v>888</v>
       </c>
     </row>
     <row r="88" spans="1:12" ht="32" x14ac:dyDescent="0.2">
@@ -7415,13 +7411,13 @@
         <v>475</v>
       </c>
       <c r="H88" s="2" t="s">
-        <v>1006</v>
+        <v>1004</v>
       </c>
       <c r="J88" s="2" t="s">
-        <v>891</v>
+        <v>889</v>
       </c>
       <c r="K88" t="s">
-        <v>892</v>
+        <v>890</v>
       </c>
     </row>
     <row r="89" spans="1:12" ht="256" customHeight="1" x14ac:dyDescent="0.2">
@@ -7448,10 +7444,10 @@
         <v>567</v>
       </c>
       <c r="K89" t="s">
-        <v>893</v>
+        <v>891</v>
       </c>
       <c r="L89" s="2" t="s">
-        <v>894</v>
+        <v>892</v>
       </c>
     </row>
     <row r="90" spans="1:12" ht="144" customHeight="1" x14ac:dyDescent="0.2">
@@ -7478,10 +7474,10 @@
         <v>568</v>
       </c>
       <c r="K90" t="s">
-        <v>895</v>
+        <v>893</v>
       </c>
       <c r="L90" s="2" t="s">
-        <v>896</v>
+        <v>894</v>
       </c>
     </row>
     <row r="91" spans="1:12" ht="112" customHeight="1" x14ac:dyDescent="0.2">
@@ -7508,10 +7504,10 @@
         <v>569</v>
       </c>
       <c r="K91" t="s">
-        <v>897</v>
+        <v>895</v>
       </c>
       <c r="L91" s="2" t="s">
-        <v>898</v>
+        <v>896</v>
       </c>
     </row>
     <row r="92" spans="1:12" ht="64" customHeight="1" x14ac:dyDescent="0.2">
@@ -7538,10 +7534,10 @@
         <v>570</v>
       </c>
       <c r="K92" t="s">
-        <v>899</v>
+        <v>897</v>
       </c>
       <c r="L92" s="2" t="s">
-        <v>900</v>
+        <v>898</v>
       </c>
     </row>
     <row r="93" spans="1:12" ht="16" x14ac:dyDescent="0.2">
@@ -7564,10 +7560,10 @@
         <v>460</v>
       </c>
       <c r="J93" s="2" t="s">
-        <v>901</v>
+        <v>899</v>
       </c>
       <c r="K93" t="s">
-        <v>902</v>
+        <v>900</v>
       </c>
     </row>
     <row r="94" spans="1:12" ht="32" x14ac:dyDescent="0.2">
@@ -7590,10 +7586,10 @@
         <v>682</v>
       </c>
       <c r="J94" s="2" t="s">
-        <v>903</v>
+        <v>901</v>
       </c>
       <c r="K94" t="s">
-        <v>904</v>
+        <v>902</v>
       </c>
     </row>
     <row r="95" spans="1:12" ht="176" customHeight="1" x14ac:dyDescent="0.2">
@@ -7620,10 +7616,10 @@
         <v>571</v>
       </c>
       <c r="K95" t="s">
-        <v>905</v>
+        <v>903</v>
       </c>
       <c r="L95" s="2" t="s">
-        <v>906</v>
+        <v>904</v>
       </c>
     </row>
     <row r="96" spans="1:12" ht="160" customHeight="1" x14ac:dyDescent="0.2">
@@ -7650,10 +7646,10 @@
         <v>572</v>
       </c>
       <c r="K96" t="s">
-        <v>907</v>
+        <v>905</v>
       </c>
       <c r="L96" s="2" t="s">
-        <v>908</v>
+        <v>906</v>
       </c>
     </row>
     <row r="97" spans="1:12" ht="112" customHeight="1" x14ac:dyDescent="0.2">
@@ -7680,10 +7676,10 @@
         <v>573</v>
       </c>
       <c r="K97" t="s">
-        <v>909</v>
+        <v>907</v>
       </c>
       <c r="L97" s="2" t="s">
-        <v>910</v>
+        <v>908</v>
       </c>
     </row>
     <row r="98" spans="1:12" ht="112" customHeight="1" x14ac:dyDescent="0.2">
@@ -7710,10 +7706,10 @@
         <v>574</v>
       </c>
       <c r="K98" t="s">
-        <v>911</v>
+        <v>909</v>
       </c>
       <c r="L98" s="2" t="s">
-        <v>912</v>
+        <v>910</v>
       </c>
     </row>
     <row r="99" spans="1:12" ht="272" customHeight="1" x14ac:dyDescent="0.2">
@@ -7740,10 +7736,10 @@
         <v>575</v>
       </c>
       <c r="K99" t="s">
-        <v>913</v>
+        <v>911</v>
       </c>
       <c r="L99" s="2" t="s">
-        <v>914</v>
+        <v>912</v>
       </c>
     </row>
     <row r="100" spans="1:12" ht="32" x14ac:dyDescent="0.2">
@@ -7763,13 +7759,13 @@
         <v>477</v>
       </c>
       <c r="H100" s="2" t="s">
-        <v>1007</v>
+        <v>1005</v>
       </c>
       <c r="J100" s="2" t="s">
-        <v>915</v>
+        <v>913</v>
       </c>
       <c r="K100" t="s">
-        <v>916</v>
+        <v>914</v>
       </c>
     </row>
     <row r="101" spans="1:12" ht="208" customHeight="1" x14ac:dyDescent="0.2">
@@ -7796,10 +7792,10 @@
         <v>576</v>
       </c>
       <c r="K101" t="s">
-        <v>917</v>
+        <v>915</v>
       </c>
       <c r="L101" s="2" t="s">
-        <v>918</v>
+        <v>916</v>
       </c>
     </row>
     <row r="102" spans="1:12" ht="112" customHeight="1" x14ac:dyDescent="0.2">
@@ -7826,10 +7822,10 @@
         <v>577</v>
       </c>
       <c r="K102" t="s">
-        <v>919</v>
+        <v>917</v>
       </c>
       <c r="L102" s="2" t="s">
-        <v>920</v>
+        <v>918</v>
       </c>
     </row>
     <row r="103" spans="1:12" ht="80" customHeight="1" x14ac:dyDescent="0.2">
@@ -7856,10 +7852,10 @@
         <v>578</v>
       </c>
       <c r="K103" t="s">
-        <v>921</v>
+        <v>919</v>
       </c>
       <c r="L103" s="2" t="s">
-        <v>922</v>
+        <v>920</v>
       </c>
     </row>
     <row r="104" spans="1:12" ht="192" customHeight="1" x14ac:dyDescent="0.2">
@@ -7886,10 +7882,10 @@
         <v>579</v>
       </c>
       <c r="K104" t="s">
-        <v>923</v>
+        <v>921</v>
       </c>
       <c r="L104" s="2" t="s">
-        <v>924</v>
+        <v>922</v>
       </c>
     </row>
     <row r="105" spans="1:12" ht="128" customHeight="1" x14ac:dyDescent="0.2">
@@ -7916,10 +7912,10 @@
         <v>580</v>
       </c>
       <c r="K105" t="s">
-        <v>925</v>
+        <v>923</v>
       </c>
       <c r="L105" s="2" t="s">
-        <v>926</v>
+        <v>924</v>
       </c>
     </row>
     <row r="106" spans="1:12" ht="96" customHeight="1" x14ac:dyDescent="0.2">
@@ -7946,10 +7942,10 @@
         <v>581</v>
       </c>
       <c r="K106" t="s">
-        <v>927</v>
+        <v>925</v>
       </c>
       <c r="L106" s="2" t="s">
-        <v>928</v>
+        <v>926</v>
       </c>
     </row>
     <row r="107" spans="1:12" ht="16" x14ac:dyDescent="0.2">
@@ -7972,10 +7968,10 @@
         <v>466</v>
       </c>
       <c r="J107" s="2" t="s">
-        <v>929</v>
+        <v>927</v>
       </c>
       <c r="K107" t="s">
-        <v>930</v>
+        <v>928</v>
       </c>
     </row>
     <row r="108" spans="1:12" ht="16" x14ac:dyDescent="0.2">
@@ -7998,10 +7994,10 @@
         <v>694</v>
       </c>
       <c r="J108" s="2" t="s">
-        <v>931</v>
+        <v>929</v>
       </c>
       <c r="K108" t="s">
-        <v>932</v>
+        <v>930</v>
       </c>
     </row>
     <row r="109" spans="1:12" ht="144" customHeight="1" x14ac:dyDescent="0.2">
@@ -8028,10 +8024,10 @@
         <v>582</v>
       </c>
       <c r="K109" t="s">
-        <v>933</v>
+        <v>931</v>
       </c>
       <c r="L109" s="2" t="s">
-        <v>934</v>
+        <v>932</v>
       </c>
     </row>
     <row r="110" spans="1:12" ht="80" customHeight="1" x14ac:dyDescent="0.2">
@@ -8058,10 +8054,10 @@
         <v>583</v>
       </c>
       <c r="K110" t="s">
-        <v>935</v>
+        <v>933</v>
       </c>
       <c r="L110" s="2" t="s">
-        <v>936</v>
+        <v>934</v>
       </c>
     </row>
     <row r="111" spans="1:12" ht="160" customHeight="1" x14ac:dyDescent="0.2">
@@ -8088,10 +8084,10 @@
         <v>584</v>
       </c>
       <c r="K111" t="s">
-        <v>937</v>
+        <v>935</v>
       </c>
       <c r="L111" s="2" t="s">
-        <v>938</v>
+        <v>936</v>
       </c>
     </row>
     <row r="112" spans="1:12" ht="80" customHeight="1" x14ac:dyDescent="0.2">
@@ -8118,10 +8114,10 @@
         <v>585</v>
       </c>
       <c r="K112" t="s">
-        <v>939</v>
+        <v>937</v>
       </c>
       <c r="L112" s="2" t="s">
-        <v>940</v>
+        <v>938</v>
       </c>
     </row>
     <row r="113" spans="1:12" ht="96" customHeight="1" x14ac:dyDescent="0.2">
@@ -8148,10 +8144,10 @@
         <v>586</v>
       </c>
       <c r="K113" t="s">
-        <v>941</v>
+        <v>939</v>
       </c>
       <c r="L113" s="2" t="s">
-        <v>942</v>
+        <v>940</v>
       </c>
     </row>
     <row r="114" spans="1:12" ht="32" x14ac:dyDescent="0.2">
@@ -8171,13 +8167,13 @@
         <v>486</v>
       </c>
       <c r="H114" t="s">
-        <v>1008</v>
+        <v>1006</v>
       </c>
       <c r="J114" s="2" t="s">
-        <v>943</v>
+        <v>941</v>
       </c>
       <c r="K114" t="s">
-        <v>944</v>
+        <v>942</v>
       </c>
     </row>
     <row r="115" spans="1:12" ht="176" customHeight="1" x14ac:dyDescent="0.2">
@@ -8204,10 +8200,10 @@
         <v>587</v>
       </c>
       <c r="K115" t="s">
-        <v>945</v>
+        <v>943</v>
       </c>
       <c r="L115" s="2" t="s">
-        <v>946</v>
+        <v>944</v>
       </c>
     </row>
     <row r="116" spans="1:12" ht="144" customHeight="1" x14ac:dyDescent="0.2">
@@ -8234,10 +8230,10 @@
         <v>588</v>
       </c>
       <c r="K116" t="s">
-        <v>947</v>
+        <v>945</v>
       </c>
       <c r="L116" s="2" t="s">
-        <v>948</v>
+        <v>946</v>
       </c>
     </row>
     <row r="117" spans="1:12" ht="80" customHeight="1" x14ac:dyDescent="0.2">
@@ -8264,10 +8260,10 @@
         <v>589</v>
       </c>
       <c r="K117" t="s">
-        <v>949</v>
+        <v>947</v>
       </c>
       <c r="L117" s="2" t="s">
-        <v>950</v>
+        <v>948</v>
       </c>
     </row>
     <row r="118" spans="1:12" ht="96" customHeight="1" x14ac:dyDescent="0.2">
@@ -8294,10 +8290,10 @@
         <v>590</v>
       </c>
       <c r="K118" t="s">
-        <v>951</v>
+        <v>949</v>
       </c>
       <c r="L118" s="2" t="s">
-        <v>952</v>
+        <v>950</v>
       </c>
     </row>
     <row r="119" spans="1:12" ht="32" x14ac:dyDescent="0.2">
@@ -8317,13 +8313,13 @@
         <v>487</v>
       </c>
       <c r="H119" t="s">
-        <v>1009</v>
+        <v>1007</v>
       </c>
       <c r="J119" s="2" t="s">
-        <v>953</v>
+        <v>951</v>
       </c>
       <c r="K119" t="s">
-        <v>954</v>
+        <v>952</v>
       </c>
     </row>
     <row r="120" spans="1:12" ht="160" customHeight="1" x14ac:dyDescent="0.2">
@@ -8350,10 +8346,10 @@
         <v>591</v>
       </c>
       <c r="K120" t="s">
-        <v>955</v>
+        <v>953</v>
       </c>
       <c r="L120" s="2" t="s">
-        <v>956</v>
+        <v>954</v>
       </c>
     </row>
     <row r="121" spans="1:12" ht="240" customHeight="1" x14ac:dyDescent="0.2">
@@ -8380,10 +8376,10 @@
         <v>592</v>
       </c>
       <c r="K121" t="s">
-        <v>957</v>
+        <v>955</v>
       </c>
       <c r="L121" s="2" t="s">
-        <v>958</v>
+        <v>956</v>
       </c>
     </row>
     <row r="122" spans="1:12" ht="16" x14ac:dyDescent="0.2">
@@ -8403,13 +8399,13 @@
         <v>488</v>
       </c>
       <c r="H122" t="s">
-        <v>1010</v>
+        <v>1008</v>
       </c>
       <c r="J122" s="2" t="s">
-        <v>959</v>
+        <v>957</v>
       </c>
       <c r="K122" t="s">
-        <v>960</v>
+        <v>958</v>
       </c>
     </row>
     <row r="123" spans="1:12" ht="208" customHeight="1" x14ac:dyDescent="0.2">
@@ -8436,10 +8432,10 @@
         <v>593</v>
       </c>
       <c r="K123" t="s">
-        <v>961</v>
+        <v>959</v>
       </c>
       <c r="L123" s="2" t="s">
-        <v>962</v>
+        <v>960</v>
       </c>
     </row>
     <row r="124" spans="1:12" ht="176" customHeight="1" x14ac:dyDescent="0.2">
@@ -8466,10 +8462,10 @@
         <v>594</v>
       </c>
       <c r="K124" t="s">
-        <v>963</v>
+        <v>961</v>
       </c>
       <c r="L124" s="2" t="s">
-        <v>964</v>
+        <v>962</v>
       </c>
     </row>
     <row r="125" spans="1:12" ht="16" x14ac:dyDescent="0.2">
@@ -8492,10 +8488,10 @@
         <v>467</v>
       </c>
       <c r="J125" s="2" t="s">
-        <v>965</v>
+        <v>963</v>
       </c>
       <c r="K125" t="s">
-        <v>966</v>
+        <v>964</v>
       </c>
     </row>
     <row r="126" spans="1:12" ht="32" x14ac:dyDescent="0.2">
@@ -8518,10 +8514,10 @@
         <v>708</v>
       </c>
       <c r="J126" s="2" t="s">
-        <v>967</v>
+        <v>965</v>
       </c>
       <c r="K126" t="s">
-        <v>968</v>
+        <v>966</v>
       </c>
     </row>
     <row r="127" spans="1:12" ht="96" customHeight="1" x14ac:dyDescent="0.2">
@@ -8548,10 +8544,10 @@
         <v>595</v>
       </c>
       <c r="K127" t="s">
-        <v>969</v>
+        <v>967</v>
       </c>
       <c r="L127" s="2" t="s">
-        <v>970</v>
+        <v>968</v>
       </c>
     </row>
     <row r="128" spans="1:12" ht="80" customHeight="1" x14ac:dyDescent="0.2">
@@ -8578,10 +8574,10 @@
         <v>596</v>
       </c>
       <c r="K128" t="s">
-        <v>971</v>
+        <v>969</v>
       </c>
       <c r="L128" s="2" t="s">
-        <v>972</v>
+        <v>970</v>
       </c>
     </row>
     <row r="129" spans="1:12" ht="64" customHeight="1" x14ac:dyDescent="0.2">
@@ -8608,10 +8604,10 @@
         <v>597</v>
       </c>
       <c r="K129" t="s">
-        <v>973</v>
+        <v>971</v>
       </c>
       <c r="L129" s="2" t="s">
-        <v>974</v>
+        <v>972</v>
       </c>
     </row>
     <row r="130" spans="1:12" ht="160" customHeight="1" x14ac:dyDescent="0.2">
@@ -8638,10 +8634,10 @@
         <v>598</v>
       </c>
       <c r="K130" t="s">
-        <v>975</v>
+        <v>973</v>
       </c>
       <c r="L130" s="2" t="s">
-        <v>976</v>
+        <v>974</v>
       </c>
     </row>
     <row r="131" spans="1:12" ht="112" customHeight="1" x14ac:dyDescent="0.2">
@@ -8668,10 +8664,10 @@
         <v>599</v>
       </c>
       <c r="K131" t="s">
-        <v>977</v>
+        <v>975</v>
       </c>
       <c r="L131" s="2" t="s">
-        <v>978</v>
+        <v>976</v>
       </c>
     </row>
     <row r="132" spans="1:12" ht="96" customHeight="1" x14ac:dyDescent="0.2">
@@ -8698,10 +8694,10 @@
         <v>600</v>
       </c>
       <c r="K132" t="s">
-        <v>979</v>
+        <v>977</v>
       </c>
       <c r="L132" s="2" t="s">
-        <v>980</v>
+        <v>978</v>
       </c>
     </row>
     <row r="133" spans="1:12" ht="32" x14ac:dyDescent="0.2">
@@ -8721,13 +8717,13 @@
         <v>490</v>
       </c>
       <c r="H133" t="s">
-        <v>1011</v>
+        <v>1009</v>
       </c>
       <c r="J133" s="2" t="s">
-        <v>981</v>
+        <v>979</v>
       </c>
       <c r="K133" t="s">
-        <v>982</v>
+        <v>980</v>
       </c>
     </row>
     <row r="134" spans="1:12" ht="192" customHeight="1" x14ac:dyDescent="0.2">
@@ -8754,10 +8750,10 @@
         <v>601</v>
       </c>
       <c r="K134" t="s">
-        <v>983</v>
+        <v>981</v>
       </c>
       <c r="L134" s="2" t="s">
-        <v>984</v>
+        <v>982</v>
       </c>
     </row>
     <row r="135" spans="1:12" ht="1" customHeight="1" x14ac:dyDescent="0.2">
@@ -8784,10 +8780,10 @@
         <v>602</v>
       </c>
       <c r="K135" t="s">
-        <v>985</v>
+        <v>983</v>
       </c>
       <c r="L135" s="2" t="s">
-        <v>986</v>
+        <v>984</v>
       </c>
     </row>
   </sheetData>
@@ -8799,8 +8795,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4B2A9460-ABFE-D94A-A339-D6A58073F6E8}">
   <dimension ref="A1:G6"/>
   <sheetViews>
-    <sheetView zoomScale="179" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" topLeftCell="F1" zoomScale="179" workbookViewId="0">
+      <selection activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -8830,10 +8826,10 @@
         <v>448</v>
       </c>
       <c r="F1" t="s">
-        <v>717</v>
+        <v>996</v>
       </c>
       <c r="G1" t="s">
-        <v>718</v>
+        <v>997</v>
       </c>
     </row>
     <row r="2" spans="1:7" ht="68" x14ac:dyDescent="0.2">
@@ -8853,10 +8849,10 @@
         <v>450</v>
       </c>
       <c r="F2" s="9" t="s">
-        <v>987</v>
+        <v>985</v>
       </c>
       <c r="G2" s="10" t="s">
-        <v>988</v>
+        <v>986</v>
       </c>
     </row>
     <row r="3" spans="1:7" ht="80" x14ac:dyDescent="0.2">
@@ -8876,10 +8872,10 @@
         <v>452</v>
       </c>
       <c r="F3" s="9" t="s">
-        <v>989</v>
+        <v>987</v>
       </c>
       <c r="G3" s="10" t="s">
-        <v>990</v>
+        <v>988</v>
       </c>
     </row>
     <row r="4" spans="1:7" ht="96" x14ac:dyDescent="0.2">
@@ -8899,10 +8895,10 @@
         <v>454</v>
       </c>
       <c r="F4" s="9" t="s">
-        <v>991</v>
+        <v>989</v>
       </c>
       <c r="G4" s="10" t="s">
-        <v>992</v>
+        <v>990</v>
       </c>
     </row>
     <row r="5" spans="1:7" ht="112" x14ac:dyDescent="0.2">
@@ -8922,10 +8918,10 @@
         <v>456</v>
       </c>
       <c r="F5" s="10" t="s">
-        <v>993</v>
+        <v>991</v>
       </c>
       <c r="G5" s="10" t="s">
-        <v>994</v>
+        <v>992</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.2">

</xml_diff>